<commit_message>
fixed bugs raised from testing
</commit_message>
<xml_diff>
--- a/public/assets/files/MFA_Bulk_Upload_Awards_Template.xlsx
+++ b/public/assets/files/MFA_Bulk_Upload_Awards_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.robinson\Documents\BEIS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1897A2-767A-4121-A166-B551B88F5083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CB8874-F192-4C90-9589-F2C640DE0837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fields </t>
-  </si>
-  <si>
-    <t>Mandatory/ optional</t>
   </si>
   <si>
     <t>Definition &amp; use</t>
@@ -726,13 +723,7 @@
     <t>ID Number</t>
   </si>
   <si>
-    <t>SPEIA Assistance Award</t>
-  </si>
-  <si>
     <t>Organisation Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This defines if the award is SPEIA Assistance or not </t>
   </si>
   <si>
     <t>This defines if the award will be linked to a MFA/SPEIA grouping number or not</t>
@@ -798,6 +789,15 @@
 If the ID type is a charity number, it must be 8 digits. It might include a dash (-) before the last digit.
 If the ID type is a VAT number, it must be 9 digits.
 If the ID type is a UTR, it must be 10 digits.</t>
+  </si>
+  <si>
+    <t>SPEI Assistance Award</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This defines if the award is SPEI Assistance or not </t>
+  </si>
+  <si>
+    <t>Mandatory / optional</t>
   </si>
 </sst>
 </file>
@@ -1410,10 +1410,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1351"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1430,31 +1430,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="33" t="s">
         <v>151</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -7247,9 +7247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7264,13 +7262,13 @@
         <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -7279,16 +7277,16 @@
     </row>
     <row r="2" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -7297,16 +7295,16 @@
     </row>
     <row r="3" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -7315,16 +7313,16 @@
     </row>
     <row r="4" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -7333,13 +7331,13 @@
     </row>
     <row r="5" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D5" s="22">
         <v>1000</v>
@@ -7351,16 +7349,16 @@
     </row>
     <row r="6" spans="1:8" ht="305.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -7369,16 +7367,16 @@
     </row>
     <row r="7" spans="1:8" ht="122.4" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -7387,16 +7385,16 @@
     </row>
     <row r="8" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -7405,16 +7403,16 @@
     </row>
     <row r="9" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -7423,16 +7421,16 @@
     </row>
     <row r="10" spans="1:8" ht="285.60000000000002" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -7531,16 +7529,16 @@
         <v>11</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="27" t="s">
-        <v>38</v>
-      </c>
       <c r="E1" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="27" t="s">
         <v>1</v>
@@ -7549,15 +7547,15 @@
         <v>12</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>16</v>
@@ -7566,62 +7564,62 @@
         <v>24</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H3" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>26</v>
@@ -7631,13 +7629,13 @@
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="C5" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>14</v>
@@ -7647,63 +7645,63 @@
         <v>20</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="28"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="29"/>
       <c r="D6" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H8" s="28"/>
     </row>
@@ -7718,57 +7716,57 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="H12" s="9"/>
     </row>
@@ -7781,10 +7779,10 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="H13" s="9"/>
     </row>
@@ -7796,7 +7794,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H14" s="9"/>
     </row>
@@ -7808,7 +7806,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" s="9"/>
     </row>
@@ -7820,7 +7818,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H16" s="9"/>
     </row>
@@ -7832,7 +7830,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H17" s="9"/>
     </row>
@@ -7856,7 +7854,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H19" s="9"/>
     </row>
@@ -7868,7 +7866,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H20" s="9"/>
     </row>
@@ -7892,7 +7890,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H22" s="9"/>
     </row>
@@ -7932,30 +7930,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="D2" s="23" t="s">
         <v>90</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -7963,7 +7961,7 @@
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -7971,7 +7969,7 @@
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -7979,7 +7977,7 @@
       <c r="B5" s="42"/>
       <c r="C5" s="42"/>
       <c r="D5" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7987,13 +7985,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -8001,7 +7999,7 @@
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
       <c r="D7" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -8009,7 +8007,7 @@
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
       <c r="D8" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -8017,7 +8015,7 @@
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="D9" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="245.4" x14ac:dyDescent="0.3">
@@ -8025,11 +8023,11 @@
         <v>1</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.4">
@@ -8037,13 +8035,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="D11" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="14"/>
     </row>
@@ -8052,11 +8050,11 @@
         <v>3</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8065,10 +8063,10 @@
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="123" x14ac:dyDescent="0.3">
@@ -8076,27 +8074,27 @@
         <v>5</v>
       </c>
       <c r="B14" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>106</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="C15" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>109</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8104,11 +8102,11 @@
         <v>6</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8116,13 +8114,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="D17" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8130,7 +8128,7 @@
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8138,7 +8136,7 @@
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
       <c r="D19" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8146,7 +8144,7 @@
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
       <c r="D20" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8154,7 +8152,7 @@
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
       <c r="D21" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8162,25 +8160,25 @@
         <v>8</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="24" t="s">
         <v>122</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>123</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="236.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8188,13 +8186,13 @@
         <v>9</v>
       </c>
       <c r="B24" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -8202,23 +8200,23 @@
         <v>10</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>128</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>129</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.3">
@@ -8226,28 +8224,28 @@
         <v>11</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="400.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="16"/>
@@ -8255,7 +8253,7 @@
     </row>
     <row r="30" spans="1:4" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="16"/>
@@ -8263,7 +8261,7 @@
     </row>
     <row r="31" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="16"/>
@@ -8271,7 +8269,7 @@
     </row>
     <row r="32" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
@@ -8279,7 +8277,7 @@
     </row>
     <row r="33" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="16"/>
@@ -8287,7 +8285,7 @@
     </row>
     <row r="34" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="16"/>
@@ -8295,7 +8293,7 @@
     </row>
     <row r="35" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="16"/>
@@ -8690,51 +8688,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -8784,6 +8737,51 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
@@ -8808,6 +8806,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
@@ -8828,22 +8842,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="2" removed="0"/>

</xml_diff>